<commit_message>
calculator: link to excel file corrected
</commit_message>
<xml_diff>
--- a/assets/excel-files/Annuity-Factors-Calculator-v.01.xlsx
+++ b/assets/excel-files/Annuity-Factors-Calculator-v.01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyau\Documents\ActuarialAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7184993-EF2D-40FA-8442-168A71C76F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54D4979-1C80-4484-BFD3-966EAADBD53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF301219-F2C0-4040-9DBA-23E8E2F8303E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{FF301219-F2C0-4040-9DBA-23E8E2F8303E}"/>
   </bookViews>
   <sheets>
     <sheet name="Annuity factor" sheetId="3" r:id="rId1"/>
@@ -19,17 +19,20 @@
     <sheet name="Lists" sheetId="4" r:id="rId4"/>
     <sheet name="Transfo" sheetId="2" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_cia_indexation_available">Transfo!$B$25</definedName>
-    <definedName name="_cia_indexation_warning">Transfo!$B$30</definedName>
+    <definedName name="_cia_indexation_available">Transfo!$B$26</definedName>
+    <definedName name="_cia_indexation_warning">Transfo!$B$31</definedName>
     <definedName name="_cia_interest_available">Transfo!$B$19</definedName>
-    <definedName name="_cia_loading">Transfo!$B$66</definedName>
-    <definedName name="_cia_qx_all_valid">Transfo!$E$68</definedName>
-    <definedName name="_cia_scale">Transfo!$B$64</definedName>
-    <definedName name="_cia_shift_age">Transfo!$B$65</definedName>
-    <definedName name="_cia_table">Transfo!$B$63</definedName>
-    <definedName name="_cia_warning">Transfo!$C$29</definedName>
-    <definedName name="_cia_year">Transfo!$B$67</definedName>
+    <definedName name="_cia_loading">Transfo!$B$71</definedName>
+    <definedName name="_cia_qx_all_valid">Transfo!$E$73</definedName>
+    <definedName name="_cia_scale">Transfo!$B$69</definedName>
+    <definedName name="_cia_shift_age">Transfo!$B$70</definedName>
+    <definedName name="_cia_table">Transfo!$B$68</definedName>
+    <definedName name="_cia_warning">Transfo!$C$30</definedName>
+    <definedName name="_cia_year">Transfo!$B$72</definedName>
     <definedName name="_colAge1">Annuitants!$C$4</definedName>
     <definedName name="_colAge2">Annuitants!$E$4</definedName>
     <definedName name="_colDtBirth1">Annuitants!$G$4</definedName>
@@ -52,8 +55,11 @@
     <definedName name="_e_error4">'Annuity factor'!$L$5</definedName>
     <definedName name="_e_error5">'Annuity factor'!$L$9</definedName>
     <definedName name="_f_dec2">Format!$B$6</definedName>
+    <definedName name="_f_dtCia">Format!$B$8</definedName>
+    <definedName name="_f_dtCiaShort">Format!$B$9</definedName>
     <definedName name="_f_language">Format!$B$5</definedName>
     <definedName name="_f_perc2">Format!$B$7</definedName>
+    <definedName name="_flag_cia_date">Transfo!$B$60</definedName>
     <definedName name="_i_ageIndexation">'Annuity factor'!$F$11</definedName>
     <definedName name="_i_cia_indexation_asked">'Annuity factor'!$F$9</definedName>
     <definedName name="_i_cia_interest_asked">'Annuity factor'!$F$5</definedName>
@@ -107,55 +113,59 @@
     <definedName name="_listQxTable">Lists!$E$2:$E$25</definedName>
     <definedName name="_listReversion">Lists!$B$2:$B$7</definedName>
     <definedName name="_listSex">Lists!$A$2:$A$3</definedName>
-    <definedName name="_r_annuityFactor">'Annuity factor'!$B$24</definedName>
-    <definedName name="_show_results">Transfo!$B$31</definedName>
+    <definedName name="_r_annuityFactor">'Annuity factor'!$B$23</definedName>
+    <definedName name="_show_results">Transfo!$B$32</definedName>
     <definedName name="_t_age1">Transfo!$C$8</definedName>
     <definedName name="_t_age2">Transfo!$C$9</definedName>
-    <definedName name="_t_ageFirstIndexMin">Transfo!$B$33</definedName>
-    <definedName name="_t_cia_indexation">Transfo!$B$59:$D$59</definedName>
-    <definedName name="_t_cia_indexation_asked">Transfo!$B$23</definedName>
-    <definedName name="_t_cia_indexation_conflict">Transfo!$B$24</definedName>
-    <definedName name="_t_cia_indexation_show">Transfo!$B$26</definedName>
-    <definedName name="_t_cia_interest">Transfo!$B$57:$D$57</definedName>
+    <definedName name="_t_ageFirstIndexMin">Transfo!$B$34</definedName>
+    <definedName name="_t_cia_indexation">Transfo!$B$64:$D$64</definedName>
+    <definedName name="_t_cia_indexation_asked">Transfo!$B$24</definedName>
+    <definedName name="_t_cia_indexation_conflict">Transfo!$B$25</definedName>
+    <definedName name="_t_cia_indexation_show">Transfo!$B$27</definedName>
+    <definedName name="_t_cia_interest">Transfo!$B$62:$D$62</definedName>
     <definedName name="_t_cia_interest_asked">Transfo!$B$17</definedName>
     <definedName name="_t_cia_interest_conflict">Transfo!$B$18</definedName>
     <definedName name="_t_cia_interest_show">Transfo!$B$20</definedName>
-    <definedName name="_t_deferred">Transfo!$B$46</definedName>
-    <definedName name="_t_due">Transfo!$B$48</definedName>
+    <definedName name="_t_deferred">Transfo!$B$47</definedName>
+    <definedName name="_t_dtCIA">Transfo!$B$56</definedName>
+    <definedName name="_t_due">Transfo!$B$49</definedName>
     <definedName name="_t_errorPerson">Transfo!$B$12</definedName>
-    <definedName name="_t_errorSomewhere">Transfo!$B$29</definedName>
-    <definedName name="_t_fracFirstIndexation">Transfo!$B$34</definedName>
-    <definedName name="_t_frequency">Transfo!$B$47</definedName>
-    <definedName name="_t_guarantee">Transfo!$B$44</definedName>
+    <definedName name="_t_errorSomewhere">Transfo!$B$30</definedName>
+    <definedName name="_t_fracFirstIndexation">Transfo!$B$35</definedName>
+    <definedName name="_t_frequency">Transfo!$B$48</definedName>
+    <definedName name="_t_guarantee">Transfo!$B$45</definedName>
     <definedName name="_t_hasReversion">Transfo!$B$14</definedName>
-    <definedName name="_t_indexation_fraction">Transfo!$B$53</definedName>
-    <definedName name="_t_indexation_max">Transfo!$B$54</definedName>
-    <definedName name="_t_indexationRate1">Transfo!$B$70</definedName>
+    <definedName name="_t_indexation_fraction">Transfo!$B$58</definedName>
+    <definedName name="_t_indexation_max">Transfo!$B$59</definedName>
+    <definedName name="_t_indexationRate1">Transfo!$B$75</definedName>
     <definedName name="_t_indexationVector">IF(_t_cia_indexation_show,_t_cia_indexation,IF(_i_indexationRate3&gt;0,_i_indexationVector3,IF(_i_indexationRate2&gt;0,_i_indexationVector2,_t_indexationRate1)))</definedName>
-    <definedName name="_t_interestRate1">Transfo!$B$70</definedName>
+    <definedName name="_t_interestRate1">Transfo!$B$75</definedName>
     <definedName name="_t_interestVector">IF(_t_cia_interest_show,_t_cia_interest,IF(_i_interestRate3&gt;0,_i_interestVector3,IF(_i_interestRate2&gt;0,_i_interestVector2,_i_interestRate1)))</definedName>
     <definedName name="_t_isIndexed">Transfo!$B$15</definedName>
-    <definedName name="_t_qxAgeValuation1">Transfo!$B$42</definedName>
-    <definedName name="_t_qxAgeValuation2">Transfo!$C$42</definedName>
-    <definedName name="_t_qxPre">Transfo!$B$49</definedName>
-    <definedName name="_t_qxProjection1">Transfo!$B$39</definedName>
-    <definedName name="_t_qxProjection2">Transfo!$C$39</definedName>
-    <definedName name="_t_qxScale1">Transfo!$B$40</definedName>
-    <definedName name="_t_qxScale2">Transfo!$C$40</definedName>
-    <definedName name="_t_qxTable1">Transfo!$B$38</definedName>
-    <definedName name="_t_qxTable2">Transfo!$C$38</definedName>
-    <definedName name="_t_qxValuationYear1">Transfo!$B$41</definedName>
-    <definedName name="_t_qxValuationYear2">Transfo!$C$41</definedName>
-    <definedName name="_t_reversion">Transfo!$B$45</definedName>
-    <definedName name="_t_sex1">Transfo!$B$37</definedName>
-    <definedName name="_t_sex2">Transfo!$C$37</definedName>
+    <definedName name="_t_qxAgeValuation1">Transfo!$B$43</definedName>
+    <definedName name="_t_qxAgeValuation2">Transfo!$C$43</definedName>
+    <definedName name="_t_qxPre">Transfo!$B$50</definedName>
+    <definedName name="_t_qxProjection1">Transfo!$B$40</definedName>
+    <definedName name="_t_qxProjection2">Transfo!$C$40</definedName>
+    <definedName name="_t_qxScale1">Transfo!$B$41</definedName>
+    <definedName name="_t_qxScale2">Transfo!$C$41</definedName>
+    <definedName name="_t_qxTable1">Transfo!$B$39</definedName>
+    <definedName name="_t_qxTable2">Transfo!$C$39</definedName>
+    <definedName name="_t_qxValuationYear1">Transfo!$B$42</definedName>
+    <definedName name="_t_qxValuationYear2">Transfo!$C$42</definedName>
+    <definedName name="_t_reversion">Transfo!$B$46</definedName>
+    <definedName name="_t_sex1">Transfo!$B$38</definedName>
+    <definedName name="_t_sex2">Transfo!$C$38</definedName>
     <definedName name="_t_sex2_temp">Transfo!$C$6</definedName>
+    <definedName name="_t_today">Transfo!$B$53</definedName>
+    <definedName name="_t_today_firstday">Transfo!#REF!</definedName>
     <definedName name="_tabFormat">Format!$D$5:$E$14</definedName>
     <definedName name="_tabFormatOffset">Format!$C$5</definedName>
     <definedName name="_tabPersons">Annuitants!$A:$I</definedName>
     <definedName name="_tabQxTableBaseYear">Lists!$E$2:$F$25</definedName>
     <definedName name="_z_idMax">MAX(Annuitants!$A:$A)</definedName>
     <definedName name="_z_idMin">MIN(Annuitants!$A:$A)</definedName>
+    <definedName name="date_cia_latest">Transfo!$B$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -235,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="155">
   <si>
     <t>ID</t>
   </si>
@@ -721,6 +731,36 @@
   <si>
     <t>Show results</t>
   </si>
+  <si>
+    <t>date_cia</t>
+  </si>
+  <si>
+    <t>_f_dtCia</t>
+  </si>
+  <si>
+    <t>_f_dtCiaShort</t>
+  </si>
+  <si>
+    <t>CIA date flagged ?</t>
+  </si>
+  <si>
+    <t>date_cia_latest</t>
+  </si>
+  <si>
+    <t>date_cia_calc</t>
+  </si>
+  <si>
+    <t>_t_today</t>
+  </si>
+  <si>
+    <t>flag date CIA ?</t>
+  </si>
+  <si>
+    <t>Workbook:</t>
+  </si>
+  <si>
+    <t>v.01</t>
+  </si>
 </sst>
 </file>
 
@@ -728,12 +768,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000%"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="yyyy/mmm"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -919,13 +959,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -1143,60 +1176,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1230,82 +1222,12 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1381,12 +1303,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="9" fontId="12" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
@@ -1399,32 +1315,11 @@
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
@@ -1466,70 +1361,245 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1548,6 +1618,88 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="RPPLimits"/>
+      <sheetName val="ProxyStat"/>
+      <sheetName val="QPPStat"/>
+      <sheetName val="CPPStat"/>
+      <sheetName val="OASStat"/>
+      <sheetName val="AWEStat"/>
+      <sheetName val="AWETNStat"/>
+      <sheetName val="AWEIPEStat"/>
+      <sheetName val="AWENEStat"/>
+      <sheetName val="AWENBStat"/>
+      <sheetName val="AWEQCStat"/>
+      <sheetName val="AWEONStat"/>
+      <sheetName val="AWEMAStat"/>
+      <sheetName val="AWESAStat"/>
+      <sheetName val="AWEALStat"/>
+      <sheetName val="AWECBStat"/>
+      <sheetName val="CIAStat"/>
+      <sheetName val="CPIStat"/>
+      <sheetName val="CPITNStat"/>
+      <sheetName val="CPIIPEStat"/>
+      <sheetName val="CPINEStat"/>
+      <sheetName val="CPINBStat"/>
+      <sheetName val="CPIQCStat"/>
+      <sheetName val="CPIONStat"/>
+      <sheetName val="CPIMAStat"/>
+      <sheetName val="CPISAStat"/>
+      <sheetName val="CPIALStat"/>
+      <sheetName val="CPICBStat"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="_lastDateCIAStat" refersTo="='CIAStat'!$K$1"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="K1">
+            <v>9</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16">
+        <row r="1">
+          <cell r="K1">
+            <v>44501</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1852,525 +2004,531 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.6328125" style="4" customWidth="1"/>
-    <col min="8" max="10" width="15.6328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="23.90625" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="4.7265625" style="66" customWidth="1"/>
+    <col min="5" max="5" width="31.453125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.6328125" style="24" customWidth="1"/>
+    <col min="8" max="10" width="15.6328125" style="25" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.90625" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="24" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="46">
-        <v>1</v>
-      </c>
-      <c r="C3" s="61" t="str" cm="1">
+      <c r="B3" s="82">
+        <v>1</v>
+      </c>
+      <c r="C3" s="49" t="str" cm="1">
         <f t="array" ref="C3">"&lt;-- "&amp;_z_idMin&amp;" ... "&amp;_z_idMax</f>
         <v>&lt;-- 1 ... 4</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="18" t="str">
+      <c r="A4" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="84" t="str">
         <f>LEFT(_d_name,20)</f>
         <v>Doe, John</v>
       </c>
-      <c r="C4" s="128" t="str">
-        <f ca="1">IF(_t_errorPerson,"Invalid data","")</f>
+      <c r="C4" s="85" t="str">
+        <f>IF(_t_errorPerson,"Invalid data","")</f>
         <v/>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="84">
         <f>_d_sex1</f>
         <v>1</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="98" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="99">
-        <v>0.05</v>
-      </c>
-      <c r="H5" s="47"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="125" t="str">
-        <f ca="1">IF(_t_cia_interest_conflict,"CIA and interest conflict",IF(AND(_i_cia_interest_asked,_d_dtCalc=0),"Dt Calc missing",IF(AND(NOT(_t_cia_interest_asked),_i_interestRate1=""),"&lt;-- Rate 1 missing",IF(OR(AND(_i_interestPeriod1&gt;0,_i_interestRate2=""),AND(_i_interestPeriod2&gt;0,_i_interestRate3="")),"&lt;-- Invalid vector",""))))</f>
+      <c r="F5" s="88" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="89"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="93" t="str">
+        <f>IF(_t_cia_interest_conflict,"CIA and interest conflict",IF(AND(_i_cia_interest_asked,_d_dtCalc=0),"Dt Calc missing",IF(AND(NOT(_t_cia_interest_asked),_i_interestRate1=""),"&lt;-- Rate 1 missing",IF(OR(AND(_i_interestPeriod1&gt;0,_i_interestRate2=""),AND(_i_interestPeriod2&gt;0,_i_interestRate3="")),"&lt;-- Invalid vector",""))))</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="20">
-        <f ca="1">_t_age1</f>
+      <c r="B6" s="94">
+        <f>_t_age1</f>
         <v>63</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="57" t="str">
-        <f ca="1">IF(_t_cia_interest_show,"CIA --&gt;","")</f>
+      <c r="E6" s="95"/>
+      <c r="F6" s="76" t="str">
+        <f ca="1">IF(_t_cia_interest_show,"CIA "&amp;TEXT(_t_dtCIA,_f_dtCiaShort)&amp;"--&gt;","")</f>
+        <v>CIA 2021-11--&gt;</v>
+      </c>
+      <c r="G6" s="96" cm="1">
+        <f t="array" aca="1" ref="G6:I6" ca="1">IF(_t_cia_interest_show,_t_cia_interest,"")</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H6" s="97">
+        <f ca="1"/>
+        <v>10</v>
+      </c>
+      <c r="I6" s="96">
+        <f ca="1"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="J6" s="98"/>
+      <c r="K6" s="99"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="84" cm="1">
+        <f t="array" ref="B7">_t_sex2_temp</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="100"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="94">
+        <f>_t_age2</f>
+        <v>60</v>
+      </c>
+      <c r="C8" s="101" t="str">
+        <f>IF(AND(_t_hasReversion,B8=""),"&lt;-- Missing","")</f>
         <v/>
       </c>
-      <c r="G6" s="56" t="str" cm="1">
-        <f t="array" aca="1" ref="G6" ca="1">IF(_t_cia_interest_show,_t_cia_interest,"")</f>
+      <c r="D8" s="100"/>
+      <c r="E8" s="86" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="83" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="102">
+        <f>IF(_d_dtCalc=0,"",_d_dtCalc)</f>
+        <v>44505</v>
+      </c>
+      <c r="E9" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="90" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="91"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="68" t="str">
+        <f>IF(_cia_indexation_warning,"Warning - CIA assumptions not used",IF(_t_cia_indexation_conflict,"CIA and indexation conflict",IF(AND(_i_cia_indexation_asked,_d_dtCalc=0),"Dt Calc missing",IF(OR(AND(_i_indexationPeriod1&gt;0,_i_indexationRate2=""),AND(_i_indexationPeriod2&gt;0,_i_indexationRate3="")),"&lt;-- Invalid vector",""))))</f>
         <v/>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="18" cm="1">
-        <f t="array" aca="1" ref="B7" ca="1">_t_sex2_temp</f>
-        <v>2</v>
-      </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="20">
-        <f ca="1">_t_age2</f>
-        <v>60</v>
-      </c>
-      <c r="C8" s="129" t="str">
-        <f ca="1">IF(AND(_t_hasReversion,B8=""),"&lt;-- Missing","")</f>
-        <v/>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="21">
-        <f ca="1">IF(_d_dtCalc=0,"",_d_dtCalc)</f>
-        <v>44509</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="124" t="str">
-        <f ca="1">IF(_cia_indexation_warning,"Warning - CIA assumptions not used",IF(_t_cia_indexation_conflict,"CIA and indexation conflict",IF(AND(_i_cia_indexation_asked,_d_dtCalc=0),"Dt Calc missing",IF(OR(AND(_i_indexationPeriod1&gt;0,_i_indexationRate2=""),AND(_i_indexationPeriod2&gt;0,_i_indexationRate3="")),"&lt;-- Invalid vector",""))))</f>
-        <v/>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E10" s="10"/>
-      <c r="F10" s="58" t="str">
-        <f ca="1">IF(_t_cia_indexation_show,"CIA --&gt;","")</f>
-        <v>CIA --&gt;</v>
-      </c>
-      <c r="G10" s="59" cm="1">
+      <c r="E10" s="87"/>
+      <c r="F10" s="127" t="str">
+        <f ca="1">IF(_t_cia_interest_show,"CIA "&amp;TEXT(_t_dtCIA,_f_dtCiaShort)&amp;"--&gt;","")</f>
+        <v>CIA 2021-11--&gt;</v>
+      </c>
+      <c r="G10" s="103" cm="1">
         <f t="array" aca="1" ref="G10:I10" ca="1">IF(_t_cia_indexation_show,_t_cia_indexation,"")</f>
         <v>1.4055899900391022E-2</v>
       </c>
-      <c r="H10" s="52">
+      <c r="H10" s="104">
         <f ca="1"/>
         <v>10</v>
       </c>
-      <c r="I10" s="59">
+      <c r="I10" s="103">
         <f ca="1"/>
         <v>2.0534488581689381E-2</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="106"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="E11" s="10" t="s">
+      <c r="B11" s="84"/>
+      <c r="E11" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="60" t="str" cm="1">
-        <f t="array" aca="1" ref="G11" ca="1">IF(_i_ageIndexation="","&lt;-- "&amp;TEXT(_t_ageFirstIndexMin+1,_f_dec2),"")</f>
+      <c r="F11" s="107"/>
+      <c r="G11" s="49" t="str" cm="1">
+        <f t="array" ref="G11">IF(_i_ageIndexation="","&lt;-- "&amp;TEXT(_t_ageFirstIndexMin+1,_f_dec2),"")</f>
         <v>&lt;-- 64.00</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="106"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="131">
-        <v>5</v>
-      </c>
-      <c r="C12" s="60" t="str">
+      <c r="B12" s="108"/>
+      <c r="C12" s="49" t="str">
         <f>IF(_i_guarantee="","&lt;-- "&amp;TEXT(_t_guarantee,_f_dec2),"")</f>
-        <v/>
-      </c>
-      <c r="E12" s="10" t="s">
+        <v>&lt;-- 0.00</v>
+      </c>
+      <c r="E12" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="45"/>
-      <c r="G12" s="60" t="str">
+      <c r="F12" s="107"/>
+      <c r="G12" s="49" t="str">
         <f>IF(_i_fracFirstIndexation="","&lt;-- "&amp;TEXT(1,_f_dec2),"")</f>
         <v>&lt;-- 1.00</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
+      <c r="K12" s="106"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="C13" s="60" t="str">
+      <c r="B13" s="109"/>
+      <c r="C13" s="49" t="str">
         <f>IF(_i_reversion="","&lt;-- "&amp;TEXT(_t_reversion,_f_perc2),"")</f>
-        <v/>
-      </c>
-      <c r="E13" s="87" t="s">
+        <v>&lt;-- 0.00%</v>
+      </c>
+      <c r="E13" s="110" t="s">
         <v>125</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="15"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="106"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="131"/>
-      <c r="C14" s="60" t="str">
+      <c r="B14" s="108"/>
+      <c r="C14" s="49" t="str">
         <f>IF(_i_deferred="","&lt;-- "&amp;TEXT(_t_deferred,_f_dec2),"")</f>
         <v>&lt;-- 0.00</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="88" t="str">
+      <c r="F14" s="91"/>
+      <c r="G14" s="44" t="str">
         <f>IF(_i_indexation_offset="","&lt;-- "&amp;TEXT(0,_f_perc2),"")</f>
         <v>&lt;-- 0.00%</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="15"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="106"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="131"/>
-      <c r="C15" s="60" t="str">
+      <c r="B15" s="108"/>
+      <c r="C15" s="49" t="str">
         <f>IF(_i_yearsPaid="","&lt;-- n/a","")</f>
         <v>&lt;-- n/a</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="87" t="s">
         <v>127</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="88" t="str">
+      <c r="F15" s="91"/>
+      <c r="G15" s="44" t="str">
         <f>IF(_i_indexation_fraction="","&lt;-- "&amp;TEXT(1,_f_perc2),"")</f>
         <v>&lt;-- 100.00%</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="15"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="106"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="60" t="str">
+      <c r="B16" s="112"/>
+      <c r="C16" s="49" t="str">
         <f>IF(_i_frequency="","&lt;-- "&amp;_t_frequency,"")</f>
         <v>&lt;-- 12</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="95" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="92"/>
-      <c r="G16" s="89" t="str">
+      <c r="F16" s="113"/>
+      <c r="G16" s="45" t="str">
         <f>IF(_i_indexation_max="","&lt;-- "&amp;TEXT(1,_f_perc2),"")</f>
         <v>&lt;-- 100.00%</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="40"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="114"/>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="60" t="str">
+      <c r="B17" s="112"/>
+      <c r="C17" s="49" t="str">
         <f>IF(_i_due="","&lt;-- "&amp;_t_due,"")</f>
         <v>&lt;-- TRUE</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="60" t="str">
+      <c r="B18" s="112"/>
+      <c r="C18" s="49" t="str">
         <f>IF(_i_qxPre="","&lt;-- "&amp;_t_qxPre,"")</f>
         <v>&lt;-- TRUE</v>
       </c>
-      <c r="E18" s="9" t="str">
-        <f ca="1">"Mortality"&amp;IF(_t_cia_interest_show," (CIA 3500)","")</f>
-        <v>Mortality</v>
-      </c>
-      <c r="F18" s="49" t="s">
+      <c r="E18" s="86" t="str">
+        <f>"Mortality"&amp;IF(_t_cia_interest_show," (CIA 3500)","")</f>
+        <v>Mortality (CIA 3500)</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="16"/>
+      <c r="H18" s="115"/>
+      <c r="I18" s="116"/>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="94" t="str">
-        <f ca="1">"&lt;-- "&amp;TEXT(_t_sex1,_f_dec2)&amp;" / "&amp;TEXT(_t_sex2,_f_dec2)</f>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="70" t="str">
+        <f>"&lt;-- "&amp;TEXT(_t_sex1,_f_dec2)&amp;" / "&amp;TEXT(_t_sex2,_f_dec2)</f>
         <v>&lt;-- 1.00 / 2.00</v>
       </c>
-      <c r="I19" s="95"/>
+      <c r="I19" s="71"/>
     </row>
     <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="94" t="str">
-        <f ca="1">"&lt;-- "&amp;_t_qxTable1&amp;" / "&amp;IF(_i_reversion=0,"none",_t_qxTable2)</f>
-        <v>&lt;-- UP94ICA / UP94ICA</v>
-      </c>
-      <c r="I20" s="94"/>
-      <c r="J20" s="126" t="str">
-        <f ca="1">IF(_cia_qx_all_valid,"","Invalid under CIA 3500")</f>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="70" t="str">
+        <f>"&lt;-- "&amp;_t_qxTable1&amp;" / "&amp;IF(_i_reversion=0,"none",_t_qxTable2)</f>
+        <v>&lt;-- CPM2014 / none</v>
+      </c>
+      <c r="I20" s="70"/>
+      <c r="J20" s="118" t="str">
+        <f>IF(_cia_qx_all_valid,"","Invalid under CIA 3500")</f>
         <v/>
       </c>
-      <c r="K20" s="127"/>
+      <c r="K20" s="119"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="94" t="str">
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="70" t="str">
         <f>"&lt;-- "&amp;TEXT(_i_qxShitAge1,"0")&amp;" / "&amp;IF(_i_reversion=0,"none",TEXT(_i_qxShitAge2,"0"))</f>
-        <v>&lt;-- 0 / 0</v>
-      </c>
-      <c r="I21" s="95"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D22" s="22"/>
-      <c r="E22" s="10" t="s">
+        <v>&lt;-- 0 / none</v>
+      </c>
+      <c r="I21" s="71"/>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D22" s="120"/>
+      <c r="E22" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="94" t="str">
+      <c r="F22" s="121"/>
+      <c r="G22" s="121"/>
+      <c r="H22" s="70" t="str">
         <f>"&lt;-- "&amp;TEXT(_i_qxLoading1,_f_perc2)&amp;" / "&amp;IF(_i_reversion=0,"none",TEXT(_i_qxLoading2,_f_perc2))</f>
-        <v>&lt;-- 0.00% / 0.00%</v>
-      </c>
-      <c r="I22" s="95"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="39"/>
-      <c r="E23" s="10" t="s">
+        <v>&lt;-- 0.00% / none</v>
+      </c>
+      <c r="I22" s="71"/>
+    </row>
+    <row r="23" spans="1:11" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="67" cm="1">
+        <f t="array" aca="1" ref="B23" ca="1">IF(_show_results,IF(_t_hasReversion,_xll.JS(_t_age1,_xll.LX(_t_sex1,_t_qxTable1,_i_qxShitAge1,_i_qxLoading1,_t_qxProjection1,_t_qxScale1,_ic_qxTableBaseYear1,_t_qxValuationYear1,_t_qxAgeValuation1),_t_interestVector,_t_age2,_xll.LX(_t_sex2,_t_qxTable2,_i_qxShitAge2,_i_qxLoading2,_t_qxProjection2,_t_qxScale2,_ic_qxTableBaseYear2,_t_qxValuationYear2,_t_qxAgeValuation2),_t_reversion,_t_guarantee,_t_deferred,_i_yearsPaid,_t_indexationVector,_i_ageIndexation,_t_frequency,_t_due,_t_qxPre,,,_t_fracFirstIndexation),_xll.JS(_t_age1,_xll.LX(_t_sex1,_t_qxTable1,_i_qxShitAge1,_i_qxLoading1,_t_qxProjection1,_t_qxScale1,_ic_qxTableBaseYear1,_t_qxValuationYear1,_t_qxAgeValuation1),_t_interestVector,,,,_t_guarantee,_t_deferred,_i_yearsPaid,_t_indexationVector,_i_ageIndexation,_t_frequency,_t_due,_t_qxPre,,,_t_fracFirstIndexation)),"")</f>
+        <v>21.439950014828657</v>
+      </c>
+      <c r="C23" s="123" t="str">
+        <f>IF(_cia_warning,"Warning - CIA",IF(_t_errorSomewhere,"Invalid input",""))</f>
+        <v/>
+      </c>
+      <c r="E23" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="94" t="str">
-        <f ca="1">"&lt;-- "&amp;IF(_t_qxScale1="","none",_t_qxScale1)&amp;" / "&amp;IF(_i_reversion=0,"none",_t_qxScale2)</f>
-        <v xml:space="preserve">&lt;-- none / </v>
-      </c>
-      <c r="I23" s="95"/>
-    </row>
-    <row r="24" spans="1:11" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="122" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="123" cm="1">
-        <f t="array" aca="1" ref="B24" ca="1">IF(_show_results,IF(_t_hasReversion,_xll.JS(_t_age1,_xll.LX(_t_sex1,_t_qxTable1,_i_qxShitAge1,_i_qxLoading1,_t_qxProjection1,_t_qxScale1,_ic_qxTableBaseYear1,_t_qxValuationYear1,_t_qxAgeValuation1),_t_interestVector,_t_age2,_xll.LX(_t_sex2,_t_qxTable2,_i_qxShitAge2,_i_qxLoading2,_t_qxProjection2,_t_qxScale2,_ic_qxTableBaseYear2,_t_qxValuationYear2,_t_qxAgeValuation2),_t_reversion,_t_guarantee,_t_deferred,_i_yearsPaid,_t_indexationVector,_i_ageIndexation,_t_frequency,_t_due,_t_qxPre,,,_t_fracFirstIndexation),_xll.JS(_t_age1,_xll.LX(_t_sex1,_t_qxTable1,_i_qxShitAge1,_i_qxLoading1,_t_qxProjection1,_t_qxScale1,_ic_qxTableBaseYear1,_t_qxValuationYear1,_t_qxAgeValuation1),_t_interestVector,,,,_t_guarantee,_t_deferred,_i_yearsPaid,_t_indexationVector,_i_ageIndexation,_t_frequency,_t_due,_t_qxPre,,,_t_fracFirstIndexation)),"")</f>
-        <v>16.361024666293847</v>
-      </c>
-      <c r="C24" s="121" t="str">
-        <f ca="1">IF(_cia_warning,"Warning - CIA",IF(_t_errorSomewhere,"Invalid input",""))</f>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="70" t="str">
+        <f>"&lt;-- "&amp;IF(_t_qxScale1="","none",_t_qxScale1)&amp;" / "&amp;IF(_i_reversion=0,"none",_t_qxScale2)</f>
+        <v>&lt;-- ECH_CPM_B / none</v>
+      </c>
+      <c r="I23" s="71"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E24" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="104">
+        <f>IF(_t_qxProjection1,VLOOKUP(_t_qxTable1,_tabQxTableBaseYear,2,FALSE),"")</f>
+        <v>2014</v>
+      </c>
+      <c r="G24" s="104" t="str">
+        <f>IF(AND(_t_hasReversion,_t_qxProjection2),VLOOKUP(_t_qxTable2,_tabQxTableBaseYear,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="52" t="str">
-        <f ca="1">IF(_t_qxProjection1,VLOOKUP(_t_qxTable1,_tabQxTableBaseYear,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G24" s="52" t="str">
-        <f ca="1">IF(AND(_t_hasReversion,_t_qxProjection2),VLOOKUP(_t_qxTable2,_tabQxTableBaseYear,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="15"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="106"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E25" s="10" t="s">
+      <c r="A25" s="81" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="124" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="124"/>
+      <c r="E25" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="94" t="str">
-        <f ca="1">IF(OR(_t_qxProjection1,_t_qxProjection2),"&lt;-- "&amp;_t_qxValuationYear1&amp;" / "&amp;_t_qxValuationYear2,"")</f>
-        <v/>
-      </c>
-      <c r="I25" s="95"/>
+      <c r="F25" s="117"/>
+      <c r="G25" s="117"/>
+      <c r="H25" s="70" t="str">
+        <f>IF(OR(_t_qxProjection1,_t_qxProjection2),"&lt;-- "&amp;_t_qxValuationYear1&amp;" / "&amp;_t_qxValuationYear2,"")</f>
+        <v>&lt;-- 2021 / 2021</v>
+      </c>
+      <c r="I25" s="71"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="117" t="str" cm="1">
+      <c r="B26" s="124" t="str" cm="1">
         <f t="array" ref="B26">"version "&amp;_xll.version_aea()</f>
         <v>version 4.5.2</v>
       </c>
-      <c r="C26" s="117"/>
-      <c r="E26" s="11" t="s">
+      <c r="C26" s="124"/>
+      <c r="E26" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="53" t="str">
-        <f ca="1">IF(_t_qxProjection1,_t_age1,"")</f>
+      <c r="F26" s="125">
+        <f>IF(_t_qxProjection1,_t_age1,"")</f>
+        <v>63</v>
+      </c>
+      <c r="G26" s="125" t="str">
+        <f>IF(AND(_t_hasReversion,_t_qxProjection2),_t_age2,"")</f>
         <v/>
       </c>
-      <c r="G26" s="53" t="str">
-        <f ca="1">IF(AND(_t_hasReversion,_t_qxProjection2),_t_age2,"")</f>
-        <v/>
-      </c>
-      <c r="H26" s="12"/>
-      <c r="I26" s="13"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="99"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E27" s="26"/>
+      <c r="E27" s="126"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2h8fJxiBLef3tWg4GgvUWpBpTfT8COEJdWQy+5f+q094rNA/81cKp+GPQo8Qk9KqcOzb12rsGJnCgA4BLDA6sw==" saltValue="tsIII6fW7K4xSwrTuBOUXA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="9">
+  <sheetProtection algorithmName="SHA-512" hashValue="hN3sYFqYmLxqJQucFLf4BXvB1Qj1HmAxeBGT2tMmyFnn2lpxOq37Nc/hZ4m/W6wTNf94Z5HHZiDhOaFhLEVymA==" saltValue="5wNXa3UrffAmGcxA1lvs3A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <mergeCells count="10">
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B26:C26"/>
@@ -2380,8 +2538,24 @@
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>_flag_cia_date</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>_flag_cia_date</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>_flag_cia_date</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations xWindow="271" yWindow="555" count="28">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be between 0 and 15" prompt="Guarantee remaining (from 0 to 15 years)." sqref="B12" xr:uid="{1254AC28-C6F8-4DC5-9414-6613E1A41AFF}">
       <formula1>0</formula1>
@@ -2500,210 +2674,209 @@
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B29" sqref="B29"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="27"/>
-    <col min="2" max="2" width="14.7265625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="28"/>
-    <col min="4" max="4" width="8.7265625" style="27"/>
-    <col min="5" max="5" width="8.7265625" style="28"/>
-    <col min="6" max="6" width="8.7265625" style="27"/>
-    <col min="7" max="9" width="11.6328125" style="64" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="6"/>
+    <col min="2" max="2" width="14.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="7"/>
+    <col min="4" max="4" width="8.7265625" style="6"/>
+    <col min="5" max="5" width="8.7265625" style="7"/>
+    <col min="6" max="6" width="8.7265625" style="6"/>
+    <col min="7" max="9" width="11.6328125" style="22" customWidth="1"/>
     <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-    </row>
-    <row r="2" spans="1:9" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A2" s="112" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+    </row>
+    <row r="2" spans="1:9" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-    </row>
-    <row r="3" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:9" s="29" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="1:9" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11">
         <f>COLUMN()</f>
         <v>2</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="11">
         <f>COLUMN()</f>
         <v>3</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="11">
         <f>COLUMN()</f>
         <v>4</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="11">
         <f>COLUMN()</f>
         <v>5</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="11">
         <f>COLUMN()</f>
         <v>6</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="11">
         <f>COLUMN()</f>
         <v>7</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="11">
         <f>COLUMN()</f>
         <v>8</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="11">
         <f>COLUMN()</f>
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="63">
-        <v>1</v>
-      </c>
-      <c r="B6" s="27" t="s">
+      <c r="A6" s="21">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="21">
         <v>63</v>
       </c>
-      <c r="D6" s="27">
-        <v>1</v>
-      </c>
-      <c r="E6" s="28">
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
         <v>60</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="6">
         <v>2</v>
       </c>
-      <c r="I6" s="64">
-        <f ca="1">TODAY()</f>
-        <v>44509</v>
+      <c r="I6" s="22">
+        <v>44505</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="27">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="7">
         <v>60</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="7">
         <v>63</v>
       </c>
-      <c r="F7" s="27">
-        <v>1</v>
-      </c>
-      <c r="I7" s="64">
-        <f ca="1">TODAY()</f>
-        <v>44509</v>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="22">
+        <f ca="1">_t_today</f>
+        <v>44510</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="27">
+      <c r="A8" s="6">
         <v>3</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="27">
-        <v>1</v>
-      </c>
-      <c r="F8" s="27">
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
         <v>2</v>
       </c>
-      <c r="G8" s="64">
+      <c r="G8" s="22">
         <v>23598</v>
       </c>
-      <c r="H8" s="64">
+      <c r="H8" s="22">
         <v>21655</v>
       </c>
-      <c r="I8" s="64">
-        <f ca="1">TODAY()</f>
-        <v>44509</v>
+      <c r="I8" s="22">
+        <f ca="1">_t_today</f>
+        <v>44510</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="27">
+      <c r="A9" s="6">
         <v>4</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="G9" s="64">
+      <c r="G9" s="22">
         <v>22743</v>
       </c>
-      <c r="I9" s="64">
-        <f ca="1">TODAY()</f>
-        <v>44509</v>
+      <c r="I9" s="22">
+        <f ca="1">_t_today</f>
+        <v>44510</v>
       </c>
     </row>
   </sheetData>
@@ -2728,7 +2901,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -2736,93 +2909,127 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="66" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" style="103" customWidth="1"/>
-    <col min="3" max="3" width="1.6328125" style="103" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6328125" style="103" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="67"/>
+    <col min="1" max="1" width="14.453125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.6328125" style="53" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.6328125" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-    </row>
-    <row r="5" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="104" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+    </row>
+    <row r="5" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="102">
+      <c r="C5" s="52">
         <f>ROW()-1</f>
         <v>4</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="106" t="s">
+      <c r="E5" s="56" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B6" s="103" t="str">
+      <c r="B6" s="53" t="str">
         <f>HLOOKUP(_f_language,_tabFormat,ROW()-_tabFormatOffset,FALSE)</f>
         <v>0.00</v>
       </c>
-      <c r="D6" s="103" t="str">
+      <c r="D6" s="53" t="str">
         <f>"0.00"</f>
         <v>0.00</v>
       </c>
-      <c r="E6" s="103" t="str">
+      <c r="E6" s="53" t="str">
         <f>"0,00"</f>
         <v>0,00</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="103" t="str">
+      <c r="B7" s="53" t="str">
         <f>HLOOKUP(_f_language,_tabFormat,ROW()-_tabFormatOffset,FALSE)</f>
         <v>0.00%</v>
       </c>
-      <c r="D7" s="103" t="str">
+      <c r="D7" s="53" t="str">
         <f>"0.00%"</f>
         <v>0.00%</v>
       </c>
-      <c r="E7" s="103" t="str">
+      <c r="E7" s="53" t="str">
         <f>"0,00%"</f>
         <v>0,00%</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="53" t="str">
+        <f>HLOOKUP(_f_language,_tabFormat,ROW()-_tabFormatOffset,FALSE)</f>
+        <v>yyyy-mmmm</v>
+      </c>
+      <c r="D8" s="53" t="str">
+        <f>"yyyy-mmmm"</f>
+        <v>yyyy-mmmm</v>
+      </c>
+      <c r="E8" s="53" t="str">
+        <f>"aaaa-mmmm"</f>
+        <v>aaaa-mmmm</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="53" t="str">
+        <f>HLOOKUP(_f_language,_tabFormat,ROW()-_tabFormatOffset,FALSE)</f>
+        <v>yyyy-mm</v>
+      </c>
+      <c r="D9" s="53" t="str">
+        <f>"yyyy-mm"</f>
+        <v>yyyy-mm</v>
+      </c>
+      <c r="E9" s="53" t="str">
+        <f>"aaaa-mm"</f>
+        <v>aaaa-mm</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="x9gWFh1n+cuZ8z+TByz5ue1YI+JXjKYONeiuGIkN4GY6F8U3XJczV15muqSPOnlFvO/KEYYGV+Zl1U5pKCSZQQ==" saltValue="bxJJNaPwMAD8T1cn0kB7Vw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="L/SwjczhFIalzLzR+BGYhZKHsT5iWFVW3cYd3WMKR+BW5tw84eAPWqeY7BDCVR9vApgO2mV5jf4FQsrfK4cF5w==" saltValue="AztbwRtDi0XK9Pmrsjib4A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
@@ -2852,329 +3059,329 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="4"/>
-    <col min="5" max="5" width="14.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="14.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="93" t="s">
+      <c r="H1" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="130"/>
-      <c r="H2" s="4" t="s">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="69"/>
+      <c r="H2" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>0.5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="b">
+      <c r="D3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="130">
+      <c r="F3" s="69">
         <v>2014</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>0.6</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>24</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="130">
+      <c r="F4" s="69">
         <v>1994</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>26</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="130">
+      <c r="F5" s="69">
         <v>1994</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="48">
+      <c r="B6" s="18">
         <v>0.75</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>52</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="130">
+      <c r="F6" s="69">
         <v>1983</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="130">
+      <c r="F7" s="69">
         <v>1983</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="130">
+      <c r="F8" s="69">
         <v>1971</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="130">
+      <c r="F9" s="69">
         <v>2014</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="130">
+      <c r="F10" s="69">
         <v>2014</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="130">
+      <c r="F11" s="69">
         <v>2014</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="130">
+      <c r="F12" s="69">
         <v>2014</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="130">
+      <c r="F13" s="69">
         <v>2014</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="130">
+      <c r="F14" s="69">
         <v>2014</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="130">
+      <c r="F15" s="69">
         <v>2014</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="130">
+      <c r="F16" s="69">
         <v>2019</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="130">
+      <c r="F17" s="69">
         <v>2017</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="130">
+      <c r="F18" s="69">
         <v>2019</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="130">
+      <c r="F19" s="69">
         <v>2018</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="130">
+      <c r="F20" s="69">
         <v>2017</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="130">
+      <c r="F21" s="69">
         <v>2019</v>
       </c>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="130">
+      <c r="F22" s="69">
         <v>2018</v>
       </c>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="130">
+      <c r="F23" s="69">
         <v>2017</v>
       </c>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="130">
+      <c r="F24" s="69">
         <v>2019</v>
       </c>
     </row>
     <row r="25" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="130">
+      <c r="F25" s="69">
         <v>2018</v>
       </c>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="130">
+      <c r="F26" s="69">
         <v>2017</v>
       </c>
     </row>
@@ -3191,733 +3398,780 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.36328125" style="65" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="66" customWidth="1"/>
-    <col min="3" max="5" width="15.6328125" style="67" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="67"/>
+    <col min="1" max="1" width="49.36328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="24" customWidth="1"/>
+    <col min="3" max="5" width="15.6328125" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="66">
+      <c r="B1" s="24">
         <f>_id</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="66" t="str">
+      <c r="A3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="str">
         <f>VLOOKUP(_id,_tabPersons,_colName,FALSE)</f>
         <v>Doe, John</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="66">
+      <c r="B4" s="24">
         <f>VLOOKUP(_id,_tabPersons,_colSex1,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="68">
+      <c r="B5" s="26">
         <f>VLOOKUP(_id,_tabPersons,_colAge1,FALSE)</f>
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="66">
+      <c r="B6" s="24">
         <f>VLOOKUP(_id,_tabPersons,_colSex2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="C6" s="85">
-        <f ca="1">IF(_t_age2="","",IF(_d_sex2=0,3-_d_sex1,_d_sex2))</f>
+      <c r="C6" s="43">
+        <f>IF(_t_age2="","",IF(_d_sex2=0,3-_d_sex1,_d_sex2))</f>
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="68">
+      <c r="B7" s="26">
         <f>VLOOKUP(_id,_tabPersons,_colAge2,FALSE)</f>
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="69">
+      <c r="B8" s="27">
         <f>VLOOKUP(_id,_tabPersons,_colDtBirth1,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="107">
-        <f ca="1">IF(AND(_d_dtBirth1&gt;0,_d_dtCalc&gt;0),YEARFRAC(_d_dtBirth1,_d_dtCalc),_d_age1)</f>
+      <c r="C8" s="57">
+        <f>IF(AND(_d_dtBirth1&gt;0,_d_dtCalc&gt;0),YEARFRAC(_d_dtBirth1,_d_dtCalc),_d_age1)</f>
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="69">
+      <c r="B9" s="27">
         <f>VLOOKUP(_id,_tabPersons,_colDtBirth2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="107">
-        <f ca="1">IF(AND(_d_age2=0,_d_dtBirth2=0),"",IF(AND(_d_dtBirth2&gt;0,_d_dtCalc&gt;0),YEARFRAC(_d_dtBirth2,_d_dtCalc),_d_age2))</f>
+      <c r="C9" s="57">
+        <f>IF(AND(_d_age2=0,_d_dtBirth2=0),"",IF(AND(_d_dtBirth2&gt;0,_d_dtCalc&gt;0),YEARFRAC(_d_dtBirth2,_d_dtCalc),_d_age2))</f>
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="69">
-        <f ca="1">VLOOKUP(_id,_tabPersons,_colDtCalc,FALSE)</f>
-        <v>44509</v>
+      <c r="B10" s="27">
+        <f>VLOOKUP(_id,_tabPersons,_colDtCalc,FALSE)</f>
+        <v>44505</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="70"/>
-      <c r="B11" s="71" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="72" t="s">
+      <c r="D11" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72" t="s">
+      <c r="E11" s="30"/>
+      <c r="F11" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="72" t="s">
+      <c r="G11" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="72" t="s">
+      <c r="H11" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="72" t="s">
+      <c r="I11" s="30" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="73" t="b">
-        <f ca="1">NOT(AND(C12:I12))</f>
+      <c r="B12" s="31" t="b">
+        <f>NOT(AND(C12:I12))</f>
         <v>0</v>
       </c>
-      <c r="C12" s="72" t="b">
+      <c r="C12" s="30" t="b">
         <f>_d_sex1&lt;&gt;0</f>
         <v>1</v>
       </c>
-      <c r="D12" s="72" t="b">
+      <c r="D12" s="30" t="b">
         <f>OR(_d_age1&lt;&gt;0,_d_dtBirth1&lt;&gt;0)</f>
         <v>1</v>
       </c>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72" t="b">
-        <f ca="1">OR(_d_age1,AND(_d_dtCalc&lt;&gt;0,_d_dtBirth1&lt;&gt;0))</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="72" t="b">
+      <c r="E12" s="30"/>
+      <c r="F12" s="30" t="b">
+        <f>OR(_d_age1,AND(_d_dtCalc&lt;&gt;0,_d_dtBirth1&lt;&gt;0))</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="30" t="b">
         <f>OR(_d_sex2&lt;&gt;0,AND(_d_age2=0,_d_dtBirth2=0))</f>
         <v>1</v>
       </c>
-      <c r="H12" s="72" t="b">
+      <c r="H12" s="30" t="b">
         <f>OR(AND(_d_sex2=0,_d_age2=0,_d_dtBirth2=0),_d_age2&lt;&gt;0,_d_dtBirth2&lt;&gt;0)</f>
         <v>1</v>
       </c>
-      <c r="I12" s="72" t="b">
-        <f ca="1">OR(_d_age2&lt;&gt;0,AND(_d_dtCalc&lt;&gt;0,_d_dtBirth2&lt;&gt;0),AND(_d_sex2=0,_d_age2=0,_d_dtBirth2=0))</f>
+      <c r="I12" s="30" t="b">
+        <f>OR(_d_age2&lt;&gt;0,AND(_d_dtCalc&lt;&gt;0,_d_dtBirth2&lt;&gt;0),AND(_d_sex2=0,_d_age2=0,_d_dtBirth2=0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="66" t="b">
+      <c r="B14" s="24" t="b">
         <f>_i_reversion&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="66" t="b">
+      <c r="B15" s="24" t="b">
         <f>OR(_i_indexationRate1&gt;0,_i_indexationRate2&gt;0,_i_indexationRate3&gt;0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="66" t="b">
+      <c r="B17" s="24" t="b">
         <f>IF(_i_cia_interest_asked="",FALSE,_i_cia_interest_asked)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="66" t="b">
+      <c r="B18" s="24" t="b">
         <f>AND(_i_cia_interest_asked,_i_interestRate1&lt;&gt;"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="66" t="b" cm="1">
-        <f t="array" aca="1" ref="B19" ca="1">AND(NOT(_t_cia_interest_conflict),_d_dtCalc&gt;=DATE(2020,12,1),_d_dtCalc&lt;_xll.FirstDayOfMonth(TODAY()))</f>
+      <c r="B19" s="24" t="b">
+        <f>AND(NOT(_t_cia_interest_conflict),_d_dtCalc&gt;=DATE(2020,12,1))</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="66" t="b">
-        <f ca="1">AND(_t_cia_interest_asked,_cia_interest_available)</f>
-        <v>0</v>
+      <c r="B20" s="24" t="b">
+        <f>AND(_t_cia_interest_asked,_cia_interest_available)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="32" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="65" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="66" t="b">
+      <c r="B24" s="24" t="b">
         <f>IF(_i_cia_indexation_asked="",FALSE,_i_cia_indexation_asked)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="65" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="66" t="b">
+      <c r="B25" s="24" t="b">
         <f>AND(_i_cia_indexation_asked,_i_indexationRate1&lt;&gt;"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="65" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="66" t="b" cm="1">
-        <f t="array" aca="1" ref="B25" ca="1">AND(NOT(_t_cia_indexation_conflict),_d_dtCalc&gt;=DATE(2020,12,1),_d_dtCalc&lt;_xll.FirstDayOfMonth(TODAY()))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="65" t="s">
+      <c r="B26" s="24" t="b">
+        <f>AND(NOT(_t_cia_indexation_conflict),_d_dtCalc&gt;=DATE(2020,12,1))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="66" t="b">
-        <f ca="1">AND(_t_cia_indexation_asked,_cia_indexation_available)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="74" t="s">
+      <c r="B27" s="24" t="b">
+        <f>AND(_t_cia_indexation_asked,_cia_indexation_available)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="70" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="75" t="b">
-        <f ca="1">OR(_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;"",_e_error5&lt;&gt;"")</f>
+      <c r="B30" s="33" t="b">
+        <f>OR(_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;"",_e_error5&lt;&gt;"")</f>
         <v>0</v>
       </c>
-      <c r="C29" s="75" t="b">
-        <f ca="1">AND(_cia_indexation_warning,NOT(OR(_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;"")))</f>
+      <c r="C30" s="33" t="b">
+        <f>AND(_cia_indexation_warning,NOT(OR(_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;"")))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="70" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="B30" s="75" t="b">
-        <f ca="1">AND(_t_cia_interest_show,_i_indexationRate1&lt;&gt;0)</f>
+      <c r="B31" s="33" t="b">
+        <f>AND(_t_cia_interest_show,_i_indexationRate1&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="70" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="B31" s="75" t="b">
-        <f ca="1">NOT(OR(_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;""))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="65" t="s">
+      <c r="B32" s="33" t="b">
+        <f>NOT(OR(_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;""))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="66">
-        <f ca="1">_t_age1+_t_deferred+IF(NOT(_t_due),1/_t_frequency,0)</f>
+      <c r="B34" s="24">
+        <f>_t_age1+_t_deferred+IF(NOT(_t_due),1/_t_frequency,0)</f>
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="65" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="66">
+      <c r="B35" s="24">
         <f>IF(_i_fracFirstIndexation="",1,_i_fracFirstIndexation)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="76" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B37" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="76" t="s">
+      <c r="C37" s="34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="65" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="66">
+      <c r="B38" s="24">
         <f>IF(_i_sex1&gt;=1,_i_sex1,_d_sex1)</f>
         <v>1</v>
       </c>
-      <c r="C37" s="66">
-        <f ca="1">IF(_i_sex2&gt;=1,_i_sex2,_t_sex2_temp)</f>
+      <c r="C38" s="24">
+        <f>IF(_i_sex2&gt;=1,_i_sex2,_t_sex2_temp)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="65" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="66" t="str">
-        <f ca="1">IF(_t_cia_interest_show,"CPM2014",IF(_i_qxTable1="","UP94ICA",_i_qxTable1))</f>
-        <v>UP94ICA</v>
-      </c>
-      <c r="C38" s="66" t="str">
-        <f ca="1">IF(_t_hasReversion,IF(_t_cia_interest_show,"CPM2014",IF(_i_qxTable2="","UP94ICA",_i_qxTable2)),"")</f>
-        <v>UP94ICA</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="65" t="s">
+      <c r="B39" s="24" t="str">
+        <f>IF(_t_cia_interest_show,"CPM2014",IF(_i_qxTable1="","UP94ICA",_i_qxTable1))</f>
+        <v>CPM2014</v>
+      </c>
+      <c r="C39" s="24" t="str">
+        <f>IF(_t_hasReversion,IF(_t_cia_interest_show,"CPM2014",IF(_i_qxTable2="","UP94ICA",_i_qxTable2)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="66" t="b">
-        <f ca="1">IF(_t_cia_interest_show,TRUE,IF(OR(_i_qxScale1="None",_i_qxScale1=""),FALSE,TRUE))</f>
+      <c r="B40" s="24" t="b">
+        <f>IF(_t_cia_interest_show,TRUE,IF(OR(_i_qxScale1="None",_i_qxScale1=""),FALSE,TRUE))</f>
+        <v>1</v>
+      </c>
+      <c r="C40" s="24" t="b">
+        <f>IF(AND(_t_hasReversion,_t_cia_interest_show),TRUE,IF(OR(_i_qxScale2="None",_i_qxScale2=""),FALSE,TRUE))</f>
         <v>0</v>
       </c>
-      <c r="C39" s="66" t="b">
-        <f ca="1">IF(AND(_t_hasReversion,_t_cia_interest_show),TRUE,IF(OR(_i_qxScale2="None",_i_qxScale2=""),FALSE,TRUE))</f>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="41" t="str">
+        <f>IF(_t_cia_interest_show,"ECH_CPM_B",IF(OR(_i_qxScale1="None",_i_qxScale1=""),"",_i_qxScale1))</f>
+        <v>ECH_CPM_B</v>
+      </c>
+      <c r="C41" s="41" t="str">
+        <f>IF(AND(_t_hasReversion,_t_cia_interest_show),"ECH_CPM_B",IF(OR(_i_qxScale2="None",_i_qxScale2=""),"",_i_qxScale2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="24">
+        <f>IF(_t_cia_interest_show,YEAR(_d_dtCalc),IF(_i_qxValuationYear1&gt;0,_i_qxValuationYear1,IF(_d_dtCalc&gt;0,YEAR(_d_dtCalc),YEAR(_t_today))))</f>
+        <v>2021</v>
+      </c>
+      <c r="C42" s="24">
+        <f>IF(_t_cia_interest_show,YEAR(_d_dtCalc),IF(_i_qxValuationYear2&gt;0,_i_qxValuationYear2,IF(_d_dtCalc&gt;0,YEAR(_d_dtCalc),YEAR(_t_today))))</f>
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="24">
+        <f>IF(_ic_qxAgeValuation1="",0,_ic_qxAgeValuation1)</f>
+        <v>63</v>
+      </c>
+      <c r="C43" s="24">
+        <f>IF(_ic_qxAgeValuation2="",0,_ic_qxAgeValuation2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="83" t="str">
-        <f ca="1">IF(_t_cia_interest_show,"ECH_CPM_B",IF(OR(_i_qxScale1="None",_i_qxScale1=""),"",_i_qxScale1))</f>
-        <v/>
-      </c>
-      <c r="C40" s="83" t="str">
-        <f ca="1">IF(AND(_t_hasReversion,_t_cia_interest_show),"ECH_CPM_B",IF(OR(_i_qxScale2="None",_i_qxScale2=""),"",_i_qxScale2))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="66">
-        <f ca="1">IF(_t_cia_interest_show,YEAR(_d_dtCalc),IF(_i_qxValuationYear1&gt;0,_i_qxValuationYear1,IF(_d_dtCalc&gt;0,YEAR(_d_dtCalc),YEAR(TODAY()))))</f>
-        <v>2021</v>
-      </c>
-      <c r="C41" s="66">
-        <f ca="1">IF(_t_cia_interest_show,YEAR(_d_dtCalc),IF(_i_qxValuationYear2&gt;0,_i_qxValuationYear2,IF(_d_dtCalc&gt;0,YEAR(_d_dtCalc),YEAR(TODAY()))))</f>
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="66">
-        <f ca="1">IF(_ic_qxAgeValuation1="",0,_ic_qxAgeValuation1)</f>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="24">
+        <f>IF(_i_guarantee="",0,_i_guarantee)</f>
         <v>0</v>
       </c>
-      <c r="C42" s="66">
-        <f ca="1">IF(_ic_qxAgeValuation2="",0,_ic_qxAgeValuation2)</f>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="24">
+        <f>IF(_i_reversion="",0,_i_reversion)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="66">
-        <f>IF(_i_guarantee="",0,_i_guarantee)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="66">
-        <f>IF(_i_reversion="",0,_i_reversion)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="77" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="66">
+      <c r="B47" s="24">
         <f>IF(_i_deferred="",0,_i_deferred)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="77" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="66">
+      <c r="B48" s="24">
         <f>IF(_i_frequency="",12,_i_frequency)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="77" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B48" s="66" t="b">
+      <c r="B49" s="24" t="b">
         <f>IF(_i_due="",TRUE,_i_due)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="77" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="66" t="b">
+      <c r="B50" s="24" t="b">
         <f>IF(_i_qxPre="",TRUE,_i_qxPre)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="65" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="78">
-        <v>36</v>
-      </c>
-      <c r="C51" s="79">
-        <v>5</v>
-      </c>
-      <c r="D51" s="79">
-        <v>37</v>
-      </c>
-      <c r="E51" s="79"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="65" t="s">
+      <c r="E52" s="37"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" s="27">
+        <f ca="1">TODAY()</f>
+        <v>44510</v>
+      </c>
+      <c r="E53" s="37"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B54" s="75" cm="1">
+        <f t="array" ref="B54">IF(_d_dtCalc&lt;&gt;0,_xll.FirstDayOfMonth(_d_dtCalc,FALSE),_xll.FirstDayOfMonth("_t_today",FALSE))</f>
+        <v>44501</v>
+      </c>
+      <c r="E54" s="37"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" s="75" cm="1">
+        <f t="array" aca="1" ref="B55" ca="1">[1]!_lastDateCIAStat</f>
+        <v>44501</v>
+      </c>
+      <c r="E55" s="37"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="75">
+        <f ca="1">IF(_d_dtCalc&gt;0,MIN(_d_dtCalc,_t_today,date_cia_latest),MIN(_t_today,date_cia_latest))</f>
+        <v>44501</v>
+      </c>
+      <c r="E56" s="37"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="B52" s="90">
+      <c r="B57" s="46">
         <f>_i_indexation_offset</f>
         <v>0</v>
       </c>
-      <c r="C52" s="79"/>
-      <c r="D52" s="79"/>
-      <c r="E52" s="79"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="65" t="s">
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="90">
+      <c r="B58" s="46">
         <f>IF(_i_indexation_fraction="",1,_i_indexation_fraction)</f>
         <v>1</v>
       </c>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="65" t="s">
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="90">
+      <c r="B59" s="46">
         <f>IF(_i_indexation_max="",1000,_i_indexation_max)</f>
         <v>1000</v>
       </c>
-      <c r="C54" s="79"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="67"/>
-      <c r="B55" s="67"/>
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-    </row>
-    <row r="56" spans="1:6" s="120" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="77"/>
-      <c r="B56" s="118"/>
-      <c r="C56" s="119"/>
-      <c r="D56" s="119"/>
-      <c r="E56" s="119"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="65" t="s">
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" s="128" t="b">
+        <f ca="1">B54&lt;&gt;date_cia_latest</f>
+        <v>0</v>
+      </c>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+    </row>
+    <row r="61" spans="1:6" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="35"/>
+      <c r="B61" s="36">
+        <v>36</v>
+      </c>
+      <c r="C61" s="37">
+        <v>5</v>
+      </c>
+      <c r="D61" s="37">
+        <v>37</v>
+      </c>
+      <c r="E61" s="65"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="B57" s="80" cm="1">
-        <f t="array" aca="1" ref="B57" ca="1">_xll.CIA(_d_dtCalc,B51)</f>
+      <c r="B62" s="38" cm="1">
+        <f t="array" aca="1" ref="B62" ca="1">_xll.CIA(_t_dtCIA,B61)</f>
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C57" s="66" cm="1">
-        <f t="array" aca="1" ref="C57" ca="1">_xll.CIA(_d_dtCalc,C51)</f>
+      <c r="C62" s="24" cm="1">
+        <f t="array" aca="1" ref="C62" ca="1">_xll.CIA(_t_dtCIA,C61)</f>
         <v>10</v>
       </c>
-      <c r="D57" s="80" cm="1">
-        <f t="array" aca="1" ref="D57" ca="1">_xll.CIA(_d_dtCalc,D51)</f>
+      <c r="D62" s="38" cm="1">
+        <f t="array" aca="1" ref="D62" ca="1">_xll.CIA(_t_dtCIA,D61)</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="E57" s="80"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B58" s="81" cm="1">
-        <f t="array" aca="1" ref="B58" ca="1">_xll.CIA(_d_dtCalc,B60)</f>
+      <c r="E62" s="38"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B63" s="39" cm="1">
+        <f t="array" aca="1" ref="B63" ca="1">_xll.CIA(_t_dtCIA,B65)</f>
         <v>1.4055899900391022E-2</v>
       </c>
-      <c r="C58" s="66"/>
-      <c r="D58" s="81" cm="1">
-        <f t="array" aca="1" ref="D58" ca="1">_xll.CIA(_d_dtCalc,D60)</f>
+      <c r="C63" s="24"/>
+      <c r="D63" s="39" cm="1">
+        <f t="array" aca="1" ref="D63" ca="1">_xll.CIA(_t_dtCIA,D65)</f>
         <v>2.0534488581689381E-2</v>
       </c>
-      <c r="E58" s="80"/>
-      <c r="F58" s="91"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="65" t="s">
+      <c r="E63" s="38"/>
+      <c r="F63" s="47"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="81" cm="1">
-        <f t="array" aca="1" ref="B59" ca="1">MAX(0,MIN(_t_indexation_max,(_xll.CIA(_d_dtCalc,B60)-_i_indexation_offset)*_t_indexation_fraction))</f>
+      <c r="B64" s="39">
+        <f ca="1">MAX(0,MIN(_t_indexation_max,(B63-_i_indexation_offset)*_t_indexation_fraction))</f>
         <v>1.4055899900391022E-2</v>
       </c>
-      <c r="C59" s="66">
-        <f ca="1">C57</f>
+      <c r="C64" s="24">
+        <f ca="1">C62</f>
         <v>10</v>
       </c>
-      <c r="D59" s="81" cm="1">
-        <f t="array" aca="1" ref="D59" ca="1">MAX(0,MIN(_t_indexation_max,(_xll.CIA(_d_dtCalc,D60)-_i_indexation_offset)*_t_indexation_fraction))</f>
+      <c r="D64" s="39">
+        <f ca="1">MAX(0,MIN(_t_indexation_max,(D63-_i_indexation_offset)*_t_indexation_fraction))</f>
         <v>2.0534488581689381E-2</v>
       </c>
-      <c r="E59" s="81"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B60" s="78">
+      <c r="E64" s="39"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B65" s="36">
         <v>38</v>
       </c>
-      <c r="C60" s="79"/>
-      <c r="D60" s="79">
+      <c r="C65" s="37"/>
+      <c r="D65" s="37">
         <v>39</v>
       </c>
-      <c r="E60" s="79"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="82"/>
-      <c r="B61" s="83"/>
-      <c r="C61" s="97" t="s">
+      <c r="E65" s="37"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="40"/>
+      <c r="B66" s="41"/>
+      <c r="C66" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="D61" s="97"/>
-      <c r="E61" s="97"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="82"/>
-      <c r="B62" s="83"/>
-      <c r="C62" s="84" t="s">
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="40"/>
+      <c r="B67" s="41"/>
+      <c r="C67" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="D62" s="84" t="s">
+      <c r="D67" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="E62" s="84" t="s">
+      <c r="E67" s="42" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="82" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B63" s="83" t="s">
+      <c r="B68" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="85" t="b">
+      <c r="C68" s="43" t="b">
         <f>OR(_i_qxTable1="",_i_qxTable1=_cia_table)</f>
         <v>1</v>
       </c>
-      <c r="D63" s="85" t="b">
+      <c r="D68" s="43" t="b">
         <f>OR(_i_qxTable2="",_i_qxTable2=_cia_table)</f>
         <v>1</v>
       </c>
-      <c r="E63" s="85" t="b">
-        <f>AND(C63:D63)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="82" t="s">
+      <c r="E68" s="43" t="b">
+        <f>AND(C68:D68)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="83" t="s">
+      <c r="B69" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="85" t="b">
+      <c r="C69" s="43" t="b">
         <f>OR(_i_qxScale1="",_i_qxScale1=_cia_scale)</f>
         <v>1</v>
       </c>
-      <c r="D64" s="85" t="b">
+      <c r="D69" s="43" t="b">
         <f>OR(_i_qxScale2="",_i_qxScale2=_cia_scale)</f>
         <v>1</v>
       </c>
-      <c r="E64" s="85" t="b">
-        <f t="shared" ref="E64:E66" si="0">AND(C64:D64)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="82" t="s">
+      <c r="E69" s="43" t="b">
+        <f t="shared" ref="E69:E71" si="0">AND(C69:D69)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="83">
+      <c r="B70" s="41">
         <v>0</v>
       </c>
-      <c r="C65" s="85" t="b">
+      <c r="C70" s="43" t="b">
         <f>OR(_i_qxShitAge1=0,_i_qxShitAge1=_cia_shift_age)</f>
         <v>1</v>
       </c>
-      <c r="D65" s="85" t="b">
+      <c r="D70" s="43" t="b">
         <f>OR(_i_qxShitAge2=0,_i_qxShitAge2=_cia_shift_age)</f>
         <v>1</v>
       </c>
-      <c r="E65" s="85" t="b">
+      <c r="E70" s="43" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="82" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="83">
+      <c r="B71" s="41">
         <v>0</v>
       </c>
-      <c r="C66" s="85" t="b">
+      <c r="C71" s="43" t="b">
         <f>OR(_i_qxLoading1=0,_i_qxLoading1=_cia_loading)</f>
         <v>1</v>
       </c>
-      <c r="D66" s="85" t="b">
+      <c r="D71" s="43" t="b">
         <f>OR(_i_qxLoading2=0,_i_qxLoading2=_cia_loading)</f>
         <v>1</v>
       </c>
-      <c r="E66" s="85" t="b">
+      <c r="E71" s="43" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="82" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B67" s="83">
-        <f ca="1">YEAR(_d_dtCalc)</f>
+      <c r="B72" s="41">
+        <f>YEAR(_d_dtCalc)</f>
         <v>2021</v>
       </c>
-      <c r="C67" s="85" t="b">
-        <f ca="1">OR(_i_qxValuationYear1="",_i_qxValuationYear1=_cia_year)</f>
-        <v>1</v>
-      </c>
-      <c r="D67" s="85" t="b">
-        <f ca="1">OR(_i_qxValuationYear2="",_i_qxValuationYear2=_cia_year)</f>
-        <v>1</v>
-      </c>
-      <c r="E67" s="85" t="b">
-        <f ca="1">AND(C67:D67)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="82" t="s">
+      <c r="C72" s="43" t="b">
+        <f>OR(_i_qxValuationYear1="",_i_qxValuationYear1=_cia_year)</f>
+        <v>1</v>
+      </c>
+      <c r="D72" s="43" t="b">
+        <f>OR(_i_qxValuationYear2="",_i_qxValuationYear2=_cia_year)</f>
+        <v>1</v>
+      </c>
+      <c r="E72" s="43" t="b">
+        <f>AND(C72:D72)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="B68" s="83"/>
-      <c r="C68" s="85"/>
-      <c r="D68" s="85"/>
-      <c r="E68" s="85" t="b">
-        <f ca="1">OR(NOT(_t_cia_interest_show),AND(E63:E67))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="65" t="s">
+      <c r="B73" s="41"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43" t="b">
+        <f>OR(NOT(_t_cia_interest_show),AND(E68:E72))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="B70" s="90">
+      <c r="B75" s="46">
         <f>IF(_i_indexationRate1="",0,_i_indexationRate1)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="fxGwWRdfdDlGye2FZMYeqrCDD4vHK6jf9xUAQiE4TCk43w/Z3qyy2/FS7T6VzFONMC0bUUYNqqiE8TNRlaKagQ==" saltValue="biIqWhaIZFyjzEVLQyy6sQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+MGQj1hSSz4h5o3Xg48QMNqkXSX7R9+az2AFZivnb0RPS6W+wIN0tDvz4l8Rx5ACNMReKdGLFB9YHdSOOfIpTQ==" saltValue="9cXOWMD1XXECZhXNMpzVFA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
-    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C66:E66"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>